<commit_message>
Updated Introduction/Methods completed Added all the codes and data files to the folder. Can publish directly from here for later..
</commit_message>
<xml_diff>
--- a/data/02_data_extraction/data_extraction_MO_checkedSD.xlsx
+++ b/data/02_data_extraction/data_extraction_MO_checkedSD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/GNM_Analysis/data/02_data_extraction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shreyadimri/Library/CloudStorage/Dropbox/GitHub_Repo/Green_Nest_Material/data/02_data_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7854270-5FD1-7E4D-B7D9-59533F62B611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7947986F-0F12-AE45-90DC-7E0827C2AB57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="76220" windowHeight="19260" xr2:uid="{2338411D-A035-6640-9B5F-097AD98E903E}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="144">
   <si>
     <t>group_ID</t>
   </si>
@@ -517,9 +517,6 @@
     <t>shared_control</t>
   </si>
   <si>
-    <t>exclude</t>
-  </si>
-  <si>
     <t>T</t>
   </si>
   <si>
@@ -530,6 +527,12 @@
   </si>
   <si>
     <t xml:space="preserve">We have combined the data for years, since the sample size for some of the cases was as low as 1 if we seperated it by years. </t>
+  </si>
+  <si>
+    <t>exclude_NA</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
 </sst>
 </file>
@@ -978,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCDDD25-569C-114E-BA1C-CFE63559CC31}">
   <dimension ref="A1:AX13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="AS2" sqref="AS2"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1286,7 +1289,7 @@
         <v>118</v>
       </c>
       <c r="AG2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH2">
         <v>-0.66300000000000003</v>
@@ -1319,10 +1322,10 @@
         <v>86</v>
       </c>
       <c r="AR2" t="s">
+        <v>140</v>
+      </c>
+      <c r="AS2" t="s">
         <v>141</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>142</v>
       </c>
       <c r="AT2" t="s">
         <v>126</v>
@@ -1438,7 +1441,7 @@
         <v>118</v>
       </c>
       <c r="AG3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH3">
         <v>-0.42899999999999999</v>
@@ -1590,7 +1593,7 @@
         <v>118</v>
       </c>
       <c r="AG4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH4">
         <v>0.66300000000000003</v>
@@ -1655,7 +1658,7 @@
         <v>86</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="E5" t="s">
         <v>113</v>
@@ -1742,7 +1745,7 @@
         <v>118</v>
       </c>
       <c r="AG5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH5">
         <v>-1.7999999999999999E-2</v>
@@ -1807,7 +1810,7 @@
         <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s">
         <v>113</v>
@@ -1894,7 +1897,7 @@
         <v>118</v>
       </c>
       <c r="AG6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH6">
         <v>-0.16300000000000001</v>
@@ -1959,7 +1962,7 @@
         <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="E7" t="s">
         <v>113</v>
@@ -2046,7 +2049,7 @@
         <v>118</v>
       </c>
       <c r="AG7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH7">
         <v>-0.10299999999999999</v>
@@ -2111,7 +2114,7 @@
         <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="E8" t="s">
         <v>113</v>
@@ -2198,7 +2201,7 @@
         <v>118</v>
       </c>
       <c r="AG8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH8">
         <v>2.8530000000000002</v>
@@ -2263,7 +2266,7 @@
         <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="E9" t="s">
         <v>113</v>
@@ -2350,7 +2353,7 @@
         <v>118</v>
       </c>
       <c r="AG9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH9">
         <v>0.86599999999999999</v>
@@ -2415,7 +2418,7 @@
         <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="E10" t="s">
         <v>113</v>
@@ -2502,7 +2505,7 @@
         <v>118</v>
       </c>
       <c r="AG10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH10">
         <v>1.607</v>
@@ -2642,10 +2645,10 @@
         <v>125</v>
       </c>
       <c r="AC11" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AD11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AE11">
         <v>1</v>
@@ -2654,7 +2657,7 @@
         <v>118</v>
       </c>
       <c r="AG11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH11">
         <v>1.0640000000000001</v>
@@ -2794,10 +2797,10 @@
         <v>125</v>
       </c>
       <c r="AC12" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AD12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AE12">
         <v>1</v>
@@ -2806,7 +2809,7 @@
         <v>118</v>
       </c>
       <c r="AG12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH12">
         <v>-0.39600000000000002</v>
@@ -2946,10 +2949,10 @@
         <v>125</v>
       </c>
       <c r="AC13" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="AD13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AE13">
         <v>1</v>
@@ -2958,7 +2961,7 @@
         <v>118</v>
       </c>
       <c r="AG13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AH13">
         <v>-1.252</v>

</xml_diff>